<commit_message>
playing around with stressor sensitivity code
</commit_message>
<xml_diff>
--- a/excel_files/trait_stressor_sens_tidy.xlsx
+++ b/excel_files/trait_stressor_sens_tidy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="420" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2380" yWindow="600" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="stressor1_name" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,6 @@
   </sheets>
   <definedNames>
     <definedName name="sens_traits" localSheetId="0">stressor1_name!$A$1:$C$119</definedName>
-    <definedName name="sens_traits" localSheetId="1">stressor2_name!$A$1:$C$119</definedName>
     <definedName name="sens_traits" localSheetId="1">stressor2_name!$A$2:$C$120</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -947,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2524,7 +2523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>

</xml_diff>